<commit_message>
Make worksheet handling dynamic and configurable.
</commit_message>
<xml_diff>
--- a/openn/tests/data/sheets/empty_if.xlsx
+++ b/openn/tests/data/sheets/empty_if.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14960"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14960" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="6" r:id="rId1"/>
     <sheet name="VALUE LISTS" sheetId="7" r:id="rId2"/>
+    <sheet name="Pages" sheetId="8" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -212,9 +213,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -332,121 +340,121 @@
   </borders>
   <cellStyleXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="15" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="15" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="15"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="15"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="15" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="15" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="15" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="15" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="15" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="15" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="15" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="15" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="15" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="15" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="15" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="15" applyFont="1"/>
   </cellXfs>
   <cellStyles count="95">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -844,7 +852,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
@@ -1112,7 +1120,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -1192,4 +1200,21 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>